<commit_message>
Aaaasss - Commented GitLatch Commit @ 2022-12-28-17-2-52-618
</commit_message>
<xml_diff>
--- a/WebEx.xlsx
+++ b/WebEx.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1D8246B-0019-4042-AD31-605CF00A99E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9394326-2FF6-D746-8694-229AE8C3069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="28260" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,14 +418,14 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="6:10">
+    <row r="5" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="6:10">
+    <row r="7" spans="6:10" x14ac:dyDescent="0.2">
       <c r="J7" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Web success - Commented GitLatch Commit @ 2022-12-28-11-34-12-892
</commit_message>
<xml_diff>
--- a/WebEx.xlsx
+++ b/WebEx.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26024"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9394326-2FF6-D746-8694-229AE8C3069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69CE90CE-0348-4EC9-B302-269F465146C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28260" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,14 +418,14 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="5" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="6:10">
       <c r="F5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="6:10">
       <c r="J7" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Aaaasss - Commented GitLatch Commit @ 2022-12-28-17-4-19-551
</commit_message>
<xml_diff>
--- a/WebEx.xlsx
+++ b/WebEx.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69CE90CE-0348-4EC9-B302-269F465146C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF1CFAFC-1CE8-F547-BAEA-9BE25789BA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="28260" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,22 +415,23 @@
   <dimension ref="F5:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="6:10">
+    <row r="5" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="6:10">
+    <row r="7" spans="6:10" x14ac:dyDescent="0.2">
       <c r="J7" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Web success - Commented GitLatch Commit @ 2022-12-28-11-35-30-423
</commit_message>
<xml_diff>
--- a/WebEx.xlsx
+++ b/WebEx.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26024"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF1CFAFC-1CE8-F547-BAEA-9BE25789BA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E367688-3EA4-4DA2-94F9-BC5C620C7E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28260" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,23 +415,22 @@
   <dimension ref="F5:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="5" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="6:10">
       <c r="F5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="6:10">
       <c r="J7" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
assssaaaaaa - Commented GitLatch Commit @ 2023-1-17-17-27-41-120
</commit_message>
<xml_diff>
--- a/WebEx.xlsx
+++ b/WebEx.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE5A25E9-7664-44D9-90C4-6D5133B19341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68E791BB-7FCA-4D77-86AB-7C341E4DE6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Test - Commented GitLatch Commit @ 2023-1-17-17-28-47-370
</commit_message>
<xml_diff>
--- a/WebEx.xlsx
+++ b/WebEx.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68E791BB-7FCA-4D77-86AB-7C341E4DE6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{033AFCD0-7F85-4CC1-8AC5-2B76D4C4B11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="F5:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>